<commit_message>
include example of the output
added the expected outcome of running the scripts with the example data
</commit_message>
<xml_diff>
--- a/conditions_file.xlsx
+++ b/conditions_file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ron Geller\Dropbox\LAB\papers\CVB3_methods_paper\final_scripts_ic50\github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ron Geller\Dropbox\LAB\papers\CVB3_methods_paper\scripts_ec_calculation\EC-calculation-scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A87BC0-2A6B-49D3-8625-DDF38CA20D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1EFFB7-1857-45FF-B36C-C73931B5DAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1740" windowWidth="27195" windowHeight="14205" tabRatio="478" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1950" windowWidth="27195" windowHeight="14205" tabRatio="478" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="47" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
   <si>
     <t>template.page</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>../experimental_template.xlsx</t>
+  </si>
+  <si>
+    <t>../example_data</t>
   </si>
 </sst>
 </file>
@@ -593,7 +596,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A5"/>
+      <selection activeCell="C3" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +657,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
         <v>47</v>
@@ -695,7 +698,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
         <v>50</v>
@@ -736,7 +739,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
         <v>52</v>
@@ -777,7 +780,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>

</xml_diff>